<commit_message>
completes merging methods and parents in one column
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -421,7 +421,7 @@
     </row>
     <row r="3">
       <c r="C3" s="2" t="n"/>
-      <c r="E3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -429,7 +429,7 @@
     </row>
     <row r="4">
       <c r="C4" s="2" t="n"/>
-      <c r="E4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -451,7 +451,7 @@
     <row r="6">
       <c r="B6" s="2" t="n"/>
       <c r="C6" s="2" t="n"/>
-      <c r="E6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -460,7 +460,7 @@
     <row r="7">
       <c r="B7" s="2" t="n"/>
       <c r="C7" s="2" t="n"/>
-      <c r="E7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -478,7 +478,7 @@
     <row r="9">
       <c r="B9" s="2" t="n"/>
       <c r="C9" s="2" t="n"/>
-      <c r="E9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
         </is>
@@ -505,7 +505,7 @@
     <row r="12">
       <c r="B12" s="2" t="n"/>
       <c r="C12" s="2" t="n"/>
-      <c r="E12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
         </is>
@@ -523,7 +523,7 @@
     <row r="14">
       <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
-      <c r="E14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -532,7 +532,7 @@
     <row r="15">
       <c r="B15" s="2" t="n"/>
       <c r="C15" s="2" t="n"/>
-      <c r="E15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
         </is>
@@ -572,7 +572,7 @@
     <row r="19">
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="n"/>
-      <c r="E19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -581,7 +581,7 @@
     <row r="20">
       <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="E20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
@@ -605,7 +605,7 @@
       <c r="A22" s="2" t="n"/>
       <c r="B22" s="2" t="n"/>
       <c r="C22" s="2" t="n"/>
-      <c r="E22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -615,7 +615,7 @@
       <c r="A23" s="2" t="n"/>
       <c r="B23" s="2" t="n"/>
       <c r="C23" s="2" t="n"/>
-      <c r="E23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
@@ -644,21 +644,21 @@
       </c>
     </row>
     <row r="25">
-      <c r="E25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="E26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="E27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>

</xml_diff>

<commit_message>
wip: classes in inheritance
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -41,7 +41,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -73,16 +73,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00FF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -375,12 +385,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,288 +398,224 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="4" min="4" width="8.4"/>
-    <col customWidth="1" max="5" min="5" width="22.8"/>
+    <col customWidth="1" max="6" min="6" width="8.4"/>
+    <col customWidth="1" max="7" min="7" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Parent</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Methods/Children</t>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Class</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="C2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>CarPollutionPermit</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="2" t="n"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>__init__</t>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>check_permit</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="C4" s="2" t="n"/>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BikePollutionPermit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="n"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="2" t="inlineStr">
+    <row r="6">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>BikePollutionPermit</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>__init__</t>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TractorPollutionPermit</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>check_permit</t>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fetch_tractor</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="n"/>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>TractorPollutionPermit</t>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>TractorPesticides</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>fetch_tractor</t>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>fetch_pesticides_permit</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>TractorPesticides</t>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Vehicle</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>TractorPesticides</t>
+      <c r="B11" s="3" t="n"/>
+      <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>mileage_calculator</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>fetch_pesticides_permit</t>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Car</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Vehicle</t>
+      <c r="B13" s="3" t="n"/>
+      <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>pollution_permit</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>__init__</t>
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Farzi</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="2" t="n"/>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>mileage_calculator</t>
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="3" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>check_farzi</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Car</t>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Bike</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Bike</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="2" t="n"/>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="2" t="n"/>
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="2" t="n"/>
-      <c r="C20" s="2" t="n"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>pollution_permit</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n"/>
-      <c r="C21" s="2" t="n"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Farzi</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n"/>
-      <c r="B22" s="2" t="n"/>
-      <c r="C22" s="2" t="n"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n"/>
-      <c r="B23" s="2" t="n"/>
-      <c r="C23" s="2" t="n"/>
-      <c r="D23" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Bike</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>pollution_permit</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>check_farzi</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E16" r:id="rId2"/>
-    <hyperlink ref="E17" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completes the first iteration of multiple inheritance plotted via arrows
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -415,7 +415,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" s="2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
@@ -427,189 +427,245 @@
       </c>
     </row>
     <row r="3">
-      <c r="E3" s="2" t="n"/>
+      <c r="B3" s="2" t="n"/>
       <c r="F3" t="inlineStr">
         <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="2" t="n"/>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>check_permit</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="D4" s="2" t="inlineStr">
+    <row r="5">
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n"/>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>BikePollutionPermit</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n"/>
-      <c r="F5" t="inlineStr">
+    <row r="6">
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="3" t="n"/>
+      <c r="F7" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" s="3" t="inlineStr">
+    <row r="8">
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="E8" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n"/>
-      <c r="F6" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>TractorPollutionPermit</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n"/>
-      <c r="F7" t="inlineStr">
+    <row r="9">
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" s="3" t="inlineStr">
+    <row r="10">
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n"/>
-      <c r="E8" s="2" t="n"/>
-      <c r="F8" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" t="inlineStr">
+    <row r="11">
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="F11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="3" t="inlineStr">
+    <row r="12">
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="D10" s="2" t="n"/>
-      <c r="E10" s="2" t="n"/>
-      <c r="F10" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
         <is>
           <t>Vehicle</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="3" t="n"/>
-      <c r="D11" s="2" t="n"/>
-      <c r="E11" s="2" t="n"/>
-      <c r="F11" t="inlineStr">
+    <row r="13">
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="n"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="3" t="n"/>
+      <c r="F14" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="3" t="inlineStr">
+    <row r="15">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="D12" s="2" t="n"/>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Car</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="3" t="n"/>
-      <c r="D13" s="2" t="n"/>
-      <c r="E13" s="2" t="n"/>
-      <c r="F13" t="inlineStr">
+    <row r="16">
+      <c r="B16" s="2" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="F17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="D14" s="2" t="n"/>
-      <c r="E14" s="2" t="n"/>
-      <c r="F14" t="inlineStr">
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="3" t="n"/>
+      <c r="F18" t="inlineStr">
         <is>
           <t>Farzi</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="3" t="n"/>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="n"/>
-      <c r="F15" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="3" t="n"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="3" t="n"/>
+      <c r="F20" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="E16" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>Bike</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="F17" t="inlineStr">
+    <row r="22">
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>pollution_permit</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="F24" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>

</xml_diff>

<commit_message>
moves ruml code and source code to study in different folders for configurational purposes
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviralsrivastava/dev/generate_uml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADC57BF-6F82-5B48-ABF8-AF4194161CAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B636AEB2-D2DD-774C-B61F-021132D73EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,9 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -481,7 +479,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
@@ -492,13 +490,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="H3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="H4" t="s">
         <v>4</v>
       </c>
@@ -507,7 +505,7 @@
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
       <c r="G5" t="s">
         <v>5</v>
       </c>
@@ -517,22 +515,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="H6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="H7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
@@ -544,16 +542,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="H9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H10" t="s">
@@ -562,17 +560,17 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="H11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D12" s="2"/>
       <c r="G12" t="s">
         <v>5</v>
       </c>
@@ -583,7 +581,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2"/>
       <c r="H13" t="s">
         <v>3</v>
       </c>
@@ -591,7 +589,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="H14" t="s">
         <v>13</v>
       </c>
@@ -599,10 +597,10 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H15" t="s">
         <v>15</v>
@@ -611,7 +609,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="H16" t="s">
         <v>3</v>
       </c>
@@ -619,7 +617,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="2"/>
       <c r="H17" t="s">
         <v>16</v>
       </c>
@@ -630,7 +628,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="F18" t="s">
         <v>1</v>
       </c>
@@ -642,7 +640,7 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="H19" t="s">
         <v>3</v>
       </c>
@@ -651,7 +649,7 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2"/>
       <c r="H20" t="s">
         <v>18</v>
       </c>
@@ -664,10 +662,10 @@
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="H21" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
ruml left side with source code in different folder works
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -380,7 +380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,8 +388,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="4" min="4" width="8.4"/>
-    <col customWidth="1" max="5" min="5" width="22.8"/>
+    <col customWidth="1" max="5" min="5" width="8.4"/>
+    <col customWidth="1" max="6" min="6" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -398,137 +398,84 @@
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Class</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
     </row>
     <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>▷</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>CarPollutionPermit</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="F3" t="inlineStr">
+      <c r="A3" s="2" t="n"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>check_permit</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n"/>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="F4" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>BikePollutionPermit</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>▷</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>BikePollutionPermit</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" s="2" t="n"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="2" t="n"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>check_permit</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
     </row>
     <row r="8">
+      <c r="A8" s="2" t="n"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
           <t>→</t>
@@ -537,83 +484,84 @@
       <c r="C8" s="2" t="n"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>▷</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>TractorPollutionPermit</t>
         </is>
       </c>
     </row>
     <row r="9">
+      <c r="A9" s="2" t="n"/>
       <c r="B9" s="2" t="n"/>
       <c r="C9" s="2" t="n"/>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
         </is>
       </c>
     </row>
     <row r="10">
+      <c r="A10" s="2" t="n"/>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>◁</t>
+          <t>←</t>
         </is>
       </c>
       <c r="C10" s="2" t="n"/>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
         </is>
       </c>
     </row>
     <row r="11">
+      <c r="A11" s="2" t="n"/>
       <c r="C11" s="2" t="n"/>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
-        </is>
-      </c>
+      <c r="A12" s="2" t="n"/>
       <c r="C12" s="2" t="n"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Car</t>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Vehicle</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
       <c r="C13" s="2" t="n"/>
-      <c r="F13" t="inlineStr">
+      <c r="D13" s="2" t="n"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>__init__</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>→</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>pollution_permit</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>→</t>
+      <c r="D14" s="2" t="n"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>mileage_calculator</t>
         </is>
       </c>
     </row>
@@ -623,120 +571,108 @@
           <t>◁</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Bike</t>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Car</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="F16" t="inlineStr">
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>__init__</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>→</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="F17" t="inlineStr">
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>→</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n"/>
-      <c r="F18" t="inlineStr">
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Farzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="n"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+      <c r="G20" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>▷</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Vehicle</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="F20" t="inlineStr">
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Bike</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>mileage_calculator</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Farzi</t>
-        </is>
-      </c>
-    </row>
     <row r="23">
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>→</t>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>pollution_permit</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>check_farzi</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>→</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
,wip: sequence diagrams, getting sorted func calls with class names.
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -440,7 +440,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
@@ -458,7 +458,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
+      <c r="B6" s="2" t="n"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -467,7 +467,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
+      <c r="B7" s="2" t="n"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -476,12 +476,12 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="2" t="n"/>
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>→</t>
@@ -496,7 +496,7 @@
     <row r="9">
       <c r="A9" s="2" t="n"/>
       <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
@@ -505,12 +505,12 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="2" t="n"/>
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
@@ -519,7 +519,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
+      <c r="B11" s="2" t="n"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
@@ -528,8 +528,8 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>→</t>
         </is>
@@ -547,8 +547,8 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
       <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
       <c r="G13" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -557,8 +557,8 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
       <c r="G14" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
@@ -571,8 +571,8 @@
           <t>◁</t>
         </is>
       </c>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="inlineStr">
+      <c r="B15" s="2" t="n"/>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
@@ -585,8 +585,8 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
       <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
       <c r="G16" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -595,8 +595,8 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
       <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
       <c r="G17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
@@ -605,8 +605,8 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
       <c r="C18" s="2" t="n"/>
-      <c r="D18" s="2" t="n"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>Farzi</t>
@@ -615,8 +615,8 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -625,8 +625,8 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
       <c r="G20" t="inlineStr">
         <is>
           <t>check_farzi</t>
@@ -639,12 +639,12 @@
           <t>◁</t>
         </is>
       </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
       <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>

</xml_diff>

<commit_message>
wip: plot red arrows for inheritance and dependency
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -380,7 +380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,8 +388,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="5" min="5" width="8.4"/>
-    <col customWidth="1" max="6" min="6" width="22.8"/>
+    <col customWidth="1" max="6" min="6" width="8.4"/>
+    <col customWidth="1" max="7" min="7" width="22.8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -399,7 +399,8 @@
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Class</t>
         </is>
@@ -408,15 +409,15 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>▷</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>CarPollutionPermit</t>
         </is>
@@ -424,7 +425,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n"/>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -432,7 +433,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n"/>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -440,17 +441,17 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>BikePollutionPermit</t>
         </is>
@@ -458,8 +459,8 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
-      <c r="G6" t="inlineStr">
+      <c r="C6" s="2" t="n"/>
+      <c r="H6" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -467,8 +468,8 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
-      <c r="G7" t="inlineStr">
+      <c r="C7" s="2" t="n"/>
+      <c r="H7" t="inlineStr">
         <is>
           <t>check_permit</t>
         </is>
@@ -476,18 +477,18 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
+      <c r="C8" s="2" t="n"/>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>TractorPollutionPermit</t>
         </is>
@@ -495,9 +496,9 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="G9" t="inlineStr">
+      <c r="C9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
+      <c r="H9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
         </is>
@@ -505,13 +506,13 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="C10" s="2" t="n"/>
+      <c r="E10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
         </is>
@@ -519,8 +520,8 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
-      <c r="G11" t="inlineStr">
+      <c r="C11" s="2" t="n"/>
+      <c r="H11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
         </is>
@@ -528,18 +529,18 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>→</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>Vehicle</t>
         </is>
@@ -547,9 +548,9 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
       <c r="C13" s="2" t="n"/>
-      <c r="G13" t="inlineStr">
+      <c r="D13" s="2" t="n"/>
+      <c r="H13" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -557,9 +558,9 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
       <c r="C14" s="2" t="n"/>
-      <c r="G14" t="inlineStr">
+      <c r="D14" s="2" t="n"/>
+      <c r="H14" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
         </is>
@@ -571,13 +572,13 @@
           <t>◁</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n"/>
-      <c r="C15" s="2" t="inlineStr">
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Car</t>
         </is>
@@ -585,9 +586,9 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
       <c r="C16" s="2" t="n"/>
-      <c r="G16" t="inlineStr">
+      <c r="D16" s="2" t="n"/>
+      <c r="H16" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -595,9 +596,9 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
       <c r="C17" s="2" t="n"/>
-      <c r="G17" t="inlineStr">
+      <c r="D17" s="2" t="n"/>
+      <c r="H17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
@@ -605,9 +606,19 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n"/>
-      <c r="B18" s="2" t="n"/>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
       <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="n"/>
       <c r="G18" t="inlineStr">
+        <is>
+          <t>▷</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>Farzi</t>
         </is>
@@ -617,7 +628,8 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="n"/>
-      <c r="G19" t="inlineStr">
+      <c r="D19" s="2" t="n"/>
+      <c r="H19" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
@@ -627,7 +639,8 @@
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="G20" t="inlineStr">
+      <c r="D20" s="2" t="n"/>
+      <c r="H20" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>
@@ -641,36 +654,41 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
           <t>←</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Bike</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>__init__</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>pollution_permit</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>check_farzi</t>
         </is>

</xml_diff>

<commit_message>
completed sequence diagram as per RUML standard. Waiting for Dr Eric's remarks on double arrows and one channel having more than one calls.
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -441,7 +441,7 @@
     </row>
     <row r="5">
       <c r="B5" s="2" t="n"/>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
@@ -459,7 +459,7 @@
     </row>
     <row r="6">
       <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -468,7 +468,7 @@
     </row>
     <row r="7">
       <c r="B7" s="2" t="n"/>
-      <c r="C7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -477,12 +477,12 @@
     </row>
     <row r="8">
       <c r="B8" s="2" t="n"/>
-      <c r="C8" s="2" t="n"/>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
+      <c r="E8" s="2" t="n"/>
       <c r="F8" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -496,7 +496,7 @@
     </row>
     <row r="9">
       <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
       <c r="H9" t="inlineStr">
         <is>
@@ -506,12 +506,12 @@
     </row>
     <row r="10">
       <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
+      <c r="E10" s="2" t="n"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
@@ -520,7 +520,7 @@
     </row>
     <row r="11">
       <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
@@ -528,91 +528,91 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
       <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Vehicle</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>mileage_calculator</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>__init__</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>pollution_permit</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n"/>
+      <c r="B18" s="2" t="n"/>
+      <c r="C18" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Vehicle</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>mileage_calculator</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>__init__</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>pollution_permit</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>⇒</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n"/>
-      <c r="C18" s="2" t="n"/>
-      <c r="D18" s="2" t="n"/>
+      <c r="E18" s="2" t="n"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>▷</t>
@@ -628,7 +628,7 @@
       <c r="A19" s="2" t="n"/>
       <c r="B19" s="2" t="n"/>
       <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
+      <c r="E19" s="2" t="n"/>
       <c r="H19" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -639,7 +639,7 @@
       <c r="A20" s="2" t="n"/>
       <c r="B20" s="2" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
+      <c r="E20" s="2" t="n"/>
       <c r="H20" t="inlineStr">
         <is>
           <t>check_farzi</t>
@@ -649,20 +649,20 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
           <t>◁</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>◁</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>

</xml_diff>

<commit_message>
added the source code for research paper
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -414,7 +414,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
@@ -431,7 +431,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n"/>
+      <c r="E3" s="2" t="n"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -439,7 +439,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
+      <c r="E4" s="2" t="n"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -447,12 +447,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
       <c r="D5" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
+      <c r="E5" s="2" t="n"/>
       <c r="F5" s="3" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -465,8 +465,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n"/>
       <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -474,8 +474,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n"/>
       <c r="D7" s="2" t="n"/>
+      <c r="E7" s="2" t="n"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -483,13 +483,13 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
       <c r="D8" s="2" t="n"/>
+      <c r="E8" s="2" t="n"/>
       <c r="F8" s="3" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -502,9 +502,9 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
       <c r="D9" s="2" t="n"/>
+      <c r="E9" s="2" t="n"/>
       <c r="H9" t="inlineStr">
         <is>
           <t>fetch_tractor</t>
@@ -512,13 +512,13 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>
       </c>
       <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
       <c r="H10" t="inlineStr">
         <is>
           <t>TractorPesticides</t>
@@ -526,8 +526,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="n"/>
       <c r="D11" s="2" t="n"/>
+      <c r="E11" s="2" t="n"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
@@ -535,13 +535,13 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n"/>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
       <c r="D12" s="2" t="n"/>
+      <c r="E12" s="2" t="n"/>
       <c r="F12" s="3" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -554,9 +554,9 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
+      <c r="B13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
+      <c r="E13" s="2" t="n"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -564,9 +564,9 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
       <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
@@ -574,17 +574,17 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>←</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>◁</t>
         </is>
       </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>←</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="n"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>Car</t>
@@ -592,9 +592,9 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
+      <c r="B16" s="2" t="n"/>
       <c r="D16" s="2" t="n"/>
+      <c r="E16" s="2" t="n"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -602,9 +602,9 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
       <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
@@ -612,14 +612,14 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="n"/>
-      <c r="C18" s="2" t="n"/>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>⇒</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n"/>
       <c r="D18" s="2" t="n"/>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>⇒</t>
-        </is>
-      </c>
+      <c r="E18" s="2" t="n"/>
       <c r="G18" s="3" t="inlineStr">
         <is>
           <t>▷</t>
@@ -633,7 +633,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n"/>
-      <c r="C19" s="2" t="n"/>
+      <c r="B19" s="2" t="n"/>
       <c r="D19" s="2" t="n"/>
       <c r="E19" s="2" t="n"/>
       <c r="H19" t="inlineStr">
@@ -644,7 +644,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n"/>
-      <c r="C20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
       <c r="H20" t="inlineStr">
@@ -659,7 +659,7 @@
           <t>◁</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>←</t>
         </is>

</xml_diff>

<commit_message>
wip: adding sys arguments
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -414,7 +414,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" s="2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
@@ -431,7 +431,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="E3" s="2" t="n"/>
+      <c r="D3" s="2" t="n"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -439,7 +439,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="E4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -447,12 +447,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n"/>
       <c r="F5" s="3" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -579,12 +579,12 @@
           <t>←</t>
         </is>
       </c>
-      <c r="D15" s="2" t="n"/>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="D15" s="2" t="inlineStr">
         <is>
           <t>◁</t>
         </is>
       </c>
+      <c r="E15" s="2" t="n"/>
       <c r="H15" t="inlineStr">
         <is>
           <t>Car</t>
@@ -666,12 +666,12 @@
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
           <t>←</t>
-        </is>
-      </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">

</xml_diff>

<commit_message>
completes function usage of generate_ruml.py
</commit_message>
<xml_diff>
--- a/Dependency_2.xlsx
+++ b/Dependency_2.xlsx
@@ -424,7 +424,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
@@ -441,7 +441,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
       <c r="H3" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -449,7 +449,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -457,12 +457,12 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
+      <c r="C5" s="2" t="n"/>
       <c r="G5" s="3" t="inlineStr">
         <is>
           <t>▷</t>
@@ -476,7 +476,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -485,7 +485,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n"/>
-      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
       <c r="H7" t="inlineStr">
         <is>
           <t>check_permit</t>
@@ -494,7 +494,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n"/>
-      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -513,7 +513,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
       <c r="E9" s="2" t="n"/>
       <c r="H9" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
       <c r="E10" s="2" t="inlineStr">
         <is>
           <t>◁</t>
@@ -537,7 +537,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n"/>
-      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
       <c r="H11" t="inlineStr">
         <is>
           <t>fetch_pesticides_permit</t>
@@ -546,12 +546,12 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
+      <c r="C12" s="2" t="n"/>
       <c r="G12" s="3" t="inlineStr">
         <is>
           <t>▷</t>
@@ -566,7 +566,7 @@
     <row r="13">
       <c r="A13" s="2" t="n"/>
       <c r="B13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -576,7 +576,7 @@
     <row r="14">
       <c r="A14" s="2" t="n"/>
       <c r="B14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
       <c r="H14" t="inlineStr">
         <is>
           <t>mileage_calculator</t>
@@ -584,15 +584,15 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>←</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n"/>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
         </is>
       </c>
       <c r="H15" s="4" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="16">
       <c r="A16" s="2" t="n"/>
       <c r="B16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
+      <c r="C16" s="2" t="n"/>
       <c r="H16" t="inlineStr">
         <is>
           <t>__init__</t>
@@ -614,7 +614,7 @@
     <row r="17">
       <c r="A17" s="2" t="n"/>
       <c r="B17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
       <c r="H17" t="inlineStr">
         <is>
           <t>pollution_permit</t>
@@ -624,12 +624,12 @@
     <row r="18">
       <c r="A18" s="2" t="n"/>
       <c r="B18" s="2" t="n"/>
-      <c r="C18" s="2" t="inlineStr">
+      <c r="C18" s="2" t="n"/>
+      <c r="D18" s="2" t="inlineStr">
         <is>
           <t>⇒</t>
         </is>
       </c>
-      <c r="D18" s="2" t="n"/>
       <c r="F18" s="3" t="inlineStr">
         <is>
           <t>⇒</t>
@@ -666,22 +666,22 @@
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>◁</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
           <t>←</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>←</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr">
-        <is>
-          <t>◁</t>
         </is>
       </c>
       <c r="H21" s="4" t="inlineStr">

</xml_diff>